<commit_message>
reset tests because of changes in symbol support
</commit_message>
<xml_diff>
--- a/HyperDbg-Testing Phase.xlsx
+++ b/HyperDbg-Testing Phase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina\Desktop\HyperDbg\testing-phase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20369BCD-C595-4A45-90FA-72E0F672CE1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4BA3B2-5659-4F13-BEE7-5EE54F520976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12900" xr2:uid="{E4F2BB4D-4D91-4D08-B645-4A180C0E6C24}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{E4F2BB4D-4D91-4D08-B645-4A180C0E6C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Commands" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
   <si>
     <t>Command</t>
   </si>
@@ -601,7 +601,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,12 +611,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -656,10 +650,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE87DE5E-1986-4A65-B106-D43404E2DB8E}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1016,29 +1006,17 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>93</v>
       </c>
@@ -1050,15 +1028,9 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>93</v>
       </c>
@@ -1070,15 +1042,9 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
         <v>93</v>
       </c>
@@ -1090,71 +1056,41 @@
       <c r="A6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="F10" s="3" t="s">
         <v>93</v>
       </c>
@@ -1163,15 +1099,9 @@
       <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="11"/>
       <c r="F11" s="3" t="s">
         <v>93</v>
       </c>
@@ -1180,15 +1110,9 @@
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="3" t="s">
         <v>93</v>
       </c>
@@ -1200,13 +1124,9 @@
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="12"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="3" t="s">
         <v>93</v>
       </c>
@@ -1218,15 +1138,9 @@
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="3" t="s">
         <v>93</v>
       </c>
@@ -1238,40 +1152,25 @@
       <c r="A15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="3" t="s">
         <v>93</v>
       </c>
@@ -1283,13 +1182,9 @@
       <c r="A18" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="12"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="3" t="s">
         <v>93</v>
       </c>
@@ -1301,13 +1196,9 @@
       <c r="A19" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="12"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="3" t="s">
         <v>93</v>
       </c>
@@ -1319,35 +1210,25 @@
       <c r="A20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="3" t="s">
         <v>93</v>
       </c>
@@ -1359,15 +1240,9 @@
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="3" t="s">
         <v>93</v>
       </c>
@@ -1379,39 +1254,25 @@
       <c r="A24" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="12"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="3" t="s">
         <v>93</v>
       </c>
@@ -1423,38 +1284,32 @@
       <c r="A27" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="3" t="s">
         <v>93</v>
       </c>
@@ -1466,15 +1321,9 @@
       <c r="A31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="3" t="s">
         <v>93</v>
       </c>
@@ -1486,15 +1335,9 @@
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="3" t="s">
         <v>93</v>
       </c>
@@ -1506,13 +1349,9 @@
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="12"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="3" t="s">
         <v>93</v>
       </c>
@@ -1524,13 +1363,9 @@
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="12"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
@@ -1538,19 +1373,15 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
@@ -1562,7 +1393,7 @@
       <c r="C37" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="3" t="s">
         <v>88</v>
       </c>
@@ -1577,7 +1408,7 @@
       <c r="C38" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="12"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="3" t="s">
         <v>88</v>
       </c>
@@ -1685,7 +1516,7 @@
       <c r="C47" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="13"/>
+      <c r="D47" s="9"/>
       <c r="E47" s="3" t="s">
         <v>88</v>
       </c>
@@ -1700,6 +1531,7 @@
       <c r="C48" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="D48" s="9"/>
       <c r="E48" s="3" t="s">
         <v>88</v>
       </c>
@@ -1714,6 +1546,7 @@
       <c r="C49" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="D49" s="9"/>
       <c r="E49" s="3" t="s">
         <v>88</v>
       </c>
@@ -1728,6 +1561,7 @@
       <c r="C50" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="D50" s="9"/>
       <c r="E50" s="3" t="s">
         <v>88</v>
       </c>
@@ -1736,12 +1570,9 @@
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
@@ -1753,7 +1584,7 @@
       <c r="C52" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="13"/>
+      <c r="D52" s="9"/>
       <c r="E52" s="3" t="s">
         <v>88</v>
       </c>
@@ -1762,32 +1593,23 @@
       <c r="A53" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D55" s="13"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="9"/>
       <c r="E55" s="3" t="s">
         <v>88</v>
       </c>
@@ -1801,7 +1623,7 @@
       </c>
       <c r="F57" s="10">
         <f xml:space="preserve"> ((COUNTA(B2:F55)) / (56 * 5))*100</f>
-        <v>56.785714285714285</v>
+        <v>25.714285714285712</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>161</v>

</xml_diff>